<commit_message>
added fix to close chrome driver at the end of the test suite
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="227">
   <si>
     <t>FirstName</t>
   </si>
@@ -706,6 +706,15 @@
   </si>
   <si>
     <t>4568939</t>
+  </si>
+  <si>
+    <t>4568957</t>
+  </si>
+  <si>
+    <t>4568958</t>
+  </si>
+  <si>
+    <t>4568959</t>
   </si>
 </sst>
 </file>
@@ -1140,8 +1149,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId6"/>
-    <hyperlink ref="C3" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId12"/>
+    <hyperlink ref="C3" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -1176,7 +1185,7 @@
         <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -1295,7 +1304,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -1522,7 +1531,7 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>196</v>
@@ -1680,7 +1689,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3657,28 +3666,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId45"/>
-    <hyperlink ref="C2" r:id="rId46"/>
-    <hyperlink ref="C3" r:id="rId47"/>
-    <hyperlink ref="C4" r:id="rId48"/>
-    <hyperlink ref="C5" r:id="rId49"/>
-    <hyperlink ref="C6" r:id="rId50"/>
-    <hyperlink ref="C7" r:id="rId51"/>
-    <hyperlink ref="C8" r:id="rId52"/>
-    <hyperlink ref="C9" r:id="rId53"/>
-    <hyperlink ref="C10" r:id="rId54"/>
-    <hyperlink ref="C11" r:id="rId55"/>
-    <hyperlink ref="C12" r:id="rId56"/>
-    <hyperlink ref="C13" r:id="rId57"/>
-    <hyperlink ref="C14" r:id="rId58"/>
-    <hyperlink ref="C15" r:id="rId59"/>
-    <hyperlink ref="C16" r:id="rId60"/>
-    <hyperlink ref="C17" r:id="rId61"/>
-    <hyperlink ref="C18" r:id="rId62"/>
-    <hyperlink ref="C19" r:id="rId63"/>
-    <hyperlink ref="C20" r:id="rId64"/>
-    <hyperlink ref="C21" r:id="rId65"/>
-    <hyperlink ref="C22" r:id="rId66"/>
+    <hyperlink ref="C1" r:id="rId111"/>
+    <hyperlink ref="C2" r:id="rId112"/>
+    <hyperlink ref="C3" r:id="rId113"/>
+    <hyperlink ref="C4" r:id="rId114"/>
+    <hyperlink ref="C5" r:id="rId115"/>
+    <hyperlink ref="C6" r:id="rId116"/>
+    <hyperlink ref="C7" r:id="rId117"/>
+    <hyperlink ref="C8" r:id="rId118"/>
+    <hyperlink ref="C9" r:id="rId119"/>
+    <hyperlink ref="C10" r:id="rId120"/>
+    <hyperlink ref="C11" r:id="rId121"/>
+    <hyperlink ref="C12" r:id="rId122"/>
+    <hyperlink ref="C13" r:id="rId123"/>
+    <hyperlink ref="C14" r:id="rId124"/>
+    <hyperlink ref="C15" r:id="rId125"/>
+    <hyperlink ref="C16" r:id="rId126"/>
+    <hyperlink ref="C17" r:id="rId127"/>
+    <hyperlink ref="C18" r:id="rId128"/>
+    <hyperlink ref="C19" r:id="rId129"/>
+    <hyperlink ref="C20" r:id="rId130"/>
+    <hyperlink ref="C21" r:id="rId131"/>
+    <hyperlink ref="C22" r:id="rId132"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
allows for script to log into LOS with a training account not the local user account
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csaenz\eclipse-workspace\Automation_Framework\src\test\resources\excel\"/>
     </mc:Choice>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="221">
   <si>
     <t>FirstName</t>
   </si>
@@ -624,15 +624,9 @@
     <t>Utah</t>
   </si>
   <si>
-    <t>Jerry</t>
-  </si>
-  <si>
     <t>Thomas</t>
   </si>
   <si>
-    <t>871</t>
-  </si>
-  <si>
     <t>Cadillac</t>
   </si>
   <si>
@@ -648,15 +642,6 @@
     <t>8185551231</t>
   </si>
   <si>
-    <t>59 Center Dr</t>
-  </si>
-  <si>
-    <t>Orlando</t>
-  </si>
-  <si>
-    <t>32835</t>
-  </si>
-  <si>
     <t>Own</t>
   </si>
   <si>
@@ -696,33 +681,29 @@
     <t>8</t>
   </si>
   <si>
-    <t>4568937</t>
-  </si>
-  <si>
-    <t>666106794</t>
-  </si>
-  <si>
-    <t>4568938</t>
-  </si>
-  <si>
-    <t>4568939</t>
-  </si>
-  <si>
-    <t>4568957</t>
-  </si>
-  <si>
-    <t>4568958</t>
-  </si>
-  <si>
-    <t>4568959</t>
+    <t>4643309</t>
+  </si>
+  <si>
+    <t>Choate</t>
+  </si>
+  <si>
+    <t>666222165</t>
+  </si>
+  <si>
+    <t>12264 NW 73RD</t>
+  </si>
+  <si>
+    <t>Parkland</t>
+  </si>
+  <si>
+    <t>33076</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1079,12 +1060,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="10.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="10.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="3" width="9.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="24.5703125" collapsed="true"/>
-    <col min="6" max="16384" style="3" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="8.7109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1149,8 +1130,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId12"/>
-    <hyperlink ref="C3" r:id="rId13"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -1167,9 +1148,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="16.140625" collapsed="true"/>
-    <col min="3" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1185,7 +1166,7 @@
         <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1204,8 +1185,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1240,14 +1221,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="10.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="10.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="3" width="9.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="24.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="19.28515625" collapsed="true"/>
-    <col min="8" max="16384" style="3" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="8.7109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1304,7 +1285,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -1315,65 +1296,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="3" width="20.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="11.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="24.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="19.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="10.140625" collapsed="true"/>
-    <col min="10" max="12" style="3" width="9.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="3" width="23.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="3" width="11.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="3" width="14.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="3" width="10.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="3" width="13.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="3" width="26.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="3" width="9.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="3" width="8.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="3" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="3" width="13.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="3" width="10.42578125" collapsed="true"/>
-    <col min="24" max="25" bestFit="true" customWidth="true" style="3" width="12.42578125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="3" width="13.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="3" width="10.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="3" width="10.0" collapsed="true"/>
-    <col min="30" max="30" style="3" width="9.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="32" max="32" style="3" width="9.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="3" width="10.42578125" collapsed="true"/>
-    <col min="34" max="36" style="3" width="9.140625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="3" width="30.42578125" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="3" width="25.140625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" style="3" width="37.0" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="3" width="37.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="3" width="28.5703125" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="3" width="37.7109375" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="3" width="21.7109375" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="3" width="11.85546875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="3" width="20.140625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" style="3" width="14.0" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="3" width="16.28515625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="3" width="18.42578125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="3" width="14.5703125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="3" width="20.5703125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="3" width="17.85546875" collapsed="true"/>
-    <col min="53" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="9.140625" style="3" collapsed="1"/>
+    <col min="13" max="13" width="23.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="26.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="12.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9.140625" style="3" collapsed="1"/>
+    <col min="31" max="31" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.140625" style="3" collapsed="1"/>
+    <col min="33" max="33" width="10.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="36" width="9.140625" style="3" collapsed="1"/>
+    <col min="37" max="37" width="30.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="25.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="37" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="37.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="28.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="37.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="21.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="11.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="20.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="14.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="14" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="18.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="20.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1496,7 +1477,7 @@
         <v>75</v>
       </c>
       <c r="AP1" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AQ1" s="3" t="s">
         <v>76</v>
@@ -1531,13 +1512,13 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>196</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>40</v>
@@ -1555,43 +1536,43 @@
         <v>6</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>93</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="O2" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>113</v>
@@ -1603,19 +1584,19 @@
         <v>24</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>6</v>
@@ -1624,7 +1605,7 @@
         <v>70</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>48</v>
@@ -1639,7 +1620,7 @@
         <v>6</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AL2" s="3" t="s">
         <v>6</v>
@@ -1660,22 +1641,22 @@
         <v>6</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="AV2" s="3" t="s">
         <v>89</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="AX2" s="3" t="s">
         <v>106</v>
@@ -1689,7 +1670,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3666,28 +3647,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId111"/>
-    <hyperlink ref="C2" r:id="rId112"/>
-    <hyperlink ref="C3" r:id="rId113"/>
-    <hyperlink ref="C4" r:id="rId114"/>
-    <hyperlink ref="C5" r:id="rId115"/>
-    <hyperlink ref="C6" r:id="rId116"/>
-    <hyperlink ref="C7" r:id="rId117"/>
-    <hyperlink ref="C8" r:id="rId118"/>
-    <hyperlink ref="C9" r:id="rId119"/>
-    <hyperlink ref="C10" r:id="rId120"/>
-    <hyperlink ref="C11" r:id="rId121"/>
-    <hyperlink ref="C12" r:id="rId122"/>
-    <hyperlink ref="C13" r:id="rId123"/>
-    <hyperlink ref="C14" r:id="rId124"/>
-    <hyperlink ref="C15" r:id="rId125"/>
-    <hyperlink ref="C16" r:id="rId126"/>
-    <hyperlink ref="C17" r:id="rId127"/>
-    <hyperlink ref="C18" r:id="rId128"/>
-    <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C20" r:id="rId130"/>
-    <hyperlink ref="C21" r:id="rId131"/>
-    <hyperlink ref="C22" r:id="rId132"/>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId8"/>
+    <hyperlink ref="C9" r:id="rId9"/>
+    <hyperlink ref="C10" r:id="rId10"/>
+    <hyperlink ref="C11" r:id="rId11"/>
+    <hyperlink ref="C12" r:id="rId12"/>
+    <hyperlink ref="C13" r:id="rId13"/>
+    <hyperlink ref="C14" r:id="rId14"/>
+    <hyperlink ref="C15" r:id="rId15"/>
+    <hyperlink ref="C16" r:id="rId16"/>
+    <hyperlink ref="C17" r:id="rId17"/>
+    <hyperlink ref="C18" r:id="rId18"/>
+    <hyperlink ref="C19" r:id="rId19"/>
+    <hyperlink ref="C20" r:id="rId20"/>
+    <hyperlink ref="C21" r:id="rId21"/>
+    <hyperlink ref="C22" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3703,15 +3684,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="3" width="29.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="17.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="13.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="17.5703125" collapsed="true"/>
-    <col min="9" max="16384" style="3" width="9.28515625" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.28515625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3782,14 +3763,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3859,17 +3840,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="21.85546875" collapsed="true"/>
-    <col min="2" max="4" style="3" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="3" width="10.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="13.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="10.42578125" collapsed="true"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" style="3" width="12.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="12.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="3" width="13.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="3" width="10.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="3" width="10.0" collapsed="true"/>
-    <col min="14" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="9.140625" style="3" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="12.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3975,20 +3956,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4094,20 +4075,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed Reason for a loan dropdown
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="269">
   <si>
     <t>FirstName</t>
   </si>
@@ -815,6 +815,36 @@
   </si>
   <si>
     <t>4643377</t>
+  </si>
+  <si>
+    <t>4643392</t>
+  </si>
+  <si>
+    <t>4643393</t>
+  </si>
+  <si>
+    <t>4643394</t>
+  </si>
+  <si>
+    <t>4643395</t>
+  </si>
+  <si>
+    <t>4643396</t>
+  </si>
+  <si>
+    <t>4643397</t>
+  </si>
+  <si>
+    <t>4643398</t>
+  </si>
+  <si>
+    <t>4643399</t>
+  </si>
+  <si>
+    <t>4643402</t>
+  </si>
+  <si>
+    <t>4643403</t>
   </si>
 </sst>
 </file>
@@ -1256,8 +1286,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId12"/>
-    <hyperlink ref="C3" r:id="rId13"/>
+    <hyperlink ref="C2" r:id="rId32"/>
+    <hyperlink ref="C3" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -1696,10 +1726,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -1818,7 +1848,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -2044,7 +2074,7 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>225</v>
@@ -2202,7 +2232,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2409,7 +2439,7 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>250</v>
@@ -2543,7 +2573,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -4520,28 +4550,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId111"/>
-    <hyperlink ref="C2" r:id="rId112"/>
-    <hyperlink ref="C3" r:id="rId113"/>
-    <hyperlink ref="C4" r:id="rId114"/>
-    <hyperlink ref="C5" r:id="rId115"/>
-    <hyperlink ref="C6" r:id="rId116"/>
-    <hyperlink ref="C7" r:id="rId117"/>
-    <hyperlink ref="C8" r:id="rId118"/>
-    <hyperlink ref="C9" r:id="rId119"/>
-    <hyperlink ref="C10" r:id="rId120"/>
-    <hyperlink ref="C11" r:id="rId121"/>
-    <hyperlink ref="C12" r:id="rId122"/>
-    <hyperlink ref="C13" r:id="rId123"/>
-    <hyperlink ref="C14" r:id="rId124"/>
-    <hyperlink ref="C15" r:id="rId125"/>
-    <hyperlink ref="C16" r:id="rId126"/>
-    <hyperlink ref="C17" r:id="rId127"/>
-    <hyperlink ref="C18" r:id="rId128"/>
-    <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C20" r:id="rId130"/>
-    <hyperlink ref="C21" r:id="rId131"/>
-    <hyperlink ref="C22" r:id="rId132"/>
+    <hyperlink ref="C1" r:id="rId331"/>
+    <hyperlink ref="C2" r:id="rId332"/>
+    <hyperlink ref="C3" r:id="rId333"/>
+    <hyperlink ref="C4" r:id="rId334"/>
+    <hyperlink ref="C5" r:id="rId335"/>
+    <hyperlink ref="C6" r:id="rId336"/>
+    <hyperlink ref="C7" r:id="rId337"/>
+    <hyperlink ref="C8" r:id="rId338"/>
+    <hyperlink ref="C9" r:id="rId339"/>
+    <hyperlink ref="C10" r:id="rId340"/>
+    <hyperlink ref="C11" r:id="rId341"/>
+    <hyperlink ref="C12" r:id="rId342"/>
+    <hyperlink ref="C13" r:id="rId343"/>
+    <hyperlink ref="C14" r:id="rId344"/>
+    <hyperlink ref="C15" r:id="rId345"/>
+    <hyperlink ref="C16" r:id="rId346"/>
+    <hyperlink ref="C17" r:id="rId347"/>
+    <hyperlink ref="C18" r:id="rId348"/>
+    <hyperlink ref="C19" r:id="rId349"/>
+    <hyperlink ref="C20" r:id="rId350"/>
+    <hyperlink ref="C21" r:id="rId351"/>
+    <hyperlink ref="C22" r:id="rId352"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
skipped test now  displays on its own tab, instead of a previous test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="270">
   <si>
     <t>FirstName</t>
   </si>
@@ -845,6 +845,9 @@
   </si>
   <si>
     <t>4643403</t>
+  </si>
+  <si>
+    <t>4643546</t>
   </si>
 </sst>
 </file>
@@ -1286,8 +1289,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId32"/>
-    <hyperlink ref="C3" r:id="rId33"/>
+    <hyperlink ref="C2" r:id="rId34"/>
+    <hyperlink ref="C3" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -1729,7 +1732,7 @@
         <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1848,7 +1851,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId17"/>
+    <hyperlink ref="C2" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -2074,7 +2077,7 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>225</v>
@@ -2232,7 +2235,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId17"/>
+    <hyperlink ref="D2" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2573,7 +2576,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId17"/>
+    <hyperlink ref="D2" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -4550,28 +4553,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId331"/>
-    <hyperlink ref="C2" r:id="rId332"/>
-    <hyperlink ref="C3" r:id="rId333"/>
-    <hyperlink ref="C4" r:id="rId334"/>
-    <hyperlink ref="C5" r:id="rId335"/>
-    <hyperlink ref="C6" r:id="rId336"/>
-    <hyperlink ref="C7" r:id="rId337"/>
-    <hyperlink ref="C8" r:id="rId338"/>
-    <hyperlink ref="C9" r:id="rId339"/>
-    <hyperlink ref="C10" r:id="rId340"/>
-    <hyperlink ref="C11" r:id="rId341"/>
-    <hyperlink ref="C12" r:id="rId342"/>
-    <hyperlink ref="C13" r:id="rId343"/>
-    <hyperlink ref="C14" r:id="rId344"/>
-    <hyperlink ref="C15" r:id="rId345"/>
-    <hyperlink ref="C16" r:id="rId346"/>
-    <hyperlink ref="C17" r:id="rId347"/>
-    <hyperlink ref="C18" r:id="rId348"/>
-    <hyperlink ref="C19" r:id="rId349"/>
-    <hyperlink ref="C20" r:id="rId350"/>
-    <hyperlink ref="C21" r:id="rId351"/>
-    <hyperlink ref="C22" r:id="rId352"/>
+    <hyperlink ref="C1" r:id="rId353"/>
+    <hyperlink ref="C2" r:id="rId354"/>
+    <hyperlink ref="C3" r:id="rId355"/>
+    <hyperlink ref="C4" r:id="rId356"/>
+    <hyperlink ref="C5" r:id="rId357"/>
+    <hyperlink ref="C6" r:id="rId358"/>
+    <hyperlink ref="C7" r:id="rId359"/>
+    <hyperlink ref="C8" r:id="rId360"/>
+    <hyperlink ref="C9" r:id="rId361"/>
+    <hyperlink ref="C10" r:id="rId362"/>
+    <hyperlink ref="C11" r:id="rId363"/>
+    <hyperlink ref="C12" r:id="rId364"/>
+    <hyperlink ref="C13" r:id="rId365"/>
+    <hyperlink ref="C14" r:id="rId366"/>
+    <hyperlink ref="C15" r:id="rId367"/>
+    <hyperlink ref="C16" r:id="rId368"/>
+    <hyperlink ref="C17" r:id="rId369"/>
+    <hyperlink ref="C18" r:id="rId370"/>
+    <hyperlink ref="C19" r:id="rId371"/>
+    <hyperlink ref="C20" r:id="rId372"/>
+    <hyperlink ref="C21" r:id="rId373"/>
+    <hyperlink ref="C22" r:id="rId374"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated chrome driver to version 78
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="272">
   <si>
     <t>FirstName</t>
   </si>
@@ -848,6 +848,12 @@
   </si>
   <si>
     <t>4643546</t>
+  </si>
+  <si>
+    <t>4643597</t>
+  </si>
+  <si>
+    <t>4643598</t>
   </si>
 </sst>
 </file>
@@ -1289,8 +1295,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId34"/>
-    <hyperlink ref="C3" r:id="rId35"/>
+    <hyperlink ref="C2" r:id="rId38"/>
+    <hyperlink ref="C3" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -1729,10 +1735,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -1851,7 +1857,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId18"/>
+    <hyperlink ref="C2" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -2077,7 +2083,7 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>225</v>
@@ -2235,7 +2241,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId18"/>
+    <hyperlink ref="D2" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2442,7 +2448,7 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>250</v>
@@ -2576,7 +2582,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId18"/>
+    <hyperlink ref="D2" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -4553,28 +4559,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId353"/>
-    <hyperlink ref="C2" r:id="rId354"/>
-    <hyperlink ref="C3" r:id="rId355"/>
-    <hyperlink ref="C4" r:id="rId356"/>
-    <hyperlink ref="C5" r:id="rId357"/>
-    <hyperlink ref="C6" r:id="rId358"/>
-    <hyperlink ref="C7" r:id="rId359"/>
-    <hyperlink ref="C8" r:id="rId360"/>
-    <hyperlink ref="C9" r:id="rId361"/>
-    <hyperlink ref="C10" r:id="rId362"/>
-    <hyperlink ref="C11" r:id="rId363"/>
-    <hyperlink ref="C12" r:id="rId364"/>
-    <hyperlink ref="C13" r:id="rId365"/>
-    <hyperlink ref="C14" r:id="rId366"/>
-    <hyperlink ref="C15" r:id="rId367"/>
-    <hyperlink ref="C16" r:id="rId368"/>
-    <hyperlink ref="C17" r:id="rId369"/>
-    <hyperlink ref="C18" r:id="rId370"/>
-    <hyperlink ref="C19" r:id="rId371"/>
-    <hyperlink ref="C20" r:id="rId372"/>
-    <hyperlink ref="C21" r:id="rId373"/>
-    <hyperlink ref="C22" r:id="rId374"/>
+    <hyperlink ref="C1" r:id="rId397"/>
+    <hyperlink ref="C2" r:id="rId398"/>
+    <hyperlink ref="C3" r:id="rId399"/>
+    <hyperlink ref="C4" r:id="rId400"/>
+    <hyperlink ref="C5" r:id="rId401"/>
+    <hyperlink ref="C6" r:id="rId402"/>
+    <hyperlink ref="C7" r:id="rId403"/>
+    <hyperlink ref="C8" r:id="rId404"/>
+    <hyperlink ref="C9" r:id="rId405"/>
+    <hyperlink ref="C10" r:id="rId406"/>
+    <hyperlink ref="C11" r:id="rId407"/>
+    <hyperlink ref="C12" r:id="rId408"/>
+    <hyperlink ref="C13" r:id="rId409"/>
+    <hyperlink ref="C14" r:id="rId410"/>
+    <hyperlink ref="C15" r:id="rId411"/>
+    <hyperlink ref="C16" r:id="rId412"/>
+    <hyperlink ref="C17" r:id="rId413"/>
+    <hyperlink ref="C18" r:id="rId414"/>
+    <hyperlink ref="C19" r:id="rId415"/>
+    <hyperlink ref="C20" r:id="rId416"/>
+    <hyperlink ref="C21" r:id="rId417"/>
+    <hyperlink ref="C22" r:id="rId418"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>